<commit_message>
task 3 excel data validation updated
</commit_message>
<xml_diff>
--- a/tasks/task3-excel-data-read/data/testData.xlsx
+++ b/tasks/task3-excel-data-read/data/testData.xlsx
@@ -471,7 +471,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +504,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>

</xml_diff>